<commit_message>
Backend - result data update
</commit_message>
<xml_diff>
--- a/Backend/car_data.xlsx
+++ b/Backend/car_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rishabhsurana/Desktop/Rishabh/CarGo.com/CarAdvisor-AI/Backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467B31F7-8951-A94A-9D11-40CEA56CBF63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C8D93F-5D34-4743-8626-8E459BD535C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="680" windowWidth="24960" windowHeight="17320" xr2:uid="{FCCC8226-0F48-1143-B6BE-845B3E6942EE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{FCCC8226-0F48-1143-B6BE-845B3E6942EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,9 +116,6 @@
     <t>Hyundai Venue</t>
   </si>
   <si>
-    <t>https://www.hyundai.com/content/dam/hyundai/in/en/data/find-a-car/Venue/Exterior/pc/venueextfront1.jpg</t>
-  </si>
-  <si>
     <t>https://www.hyundai.com/in/en/find-a-car/venue/highlights</t>
   </si>
   <si>
@@ -284,12 +281,6 @@
     <t>Hyundai EXTER</t>
   </si>
   <si>
-    <t>Hyundai EXTER VENUE N LINE</t>
-  </si>
-  <si>
-    <t>https://www.hyundai.com/content/dam/hyundai/in/en/data/find-a-car/Exter/exterior/exterfront_pc_1.jpg</t>
-  </si>
-  <si>
     <t>https://www.hyundai.com/in/en/find-a-car/exter/</t>
   </si>
   <si>
@@ -318,9 +309,6 @@
   </si>
   <si>
     <t>Hyundai CRETA N Line dominates every terrain under its wheels.</t>
-  </si>
-  <si>
-    <t>https://www.hyundai.com/content/dam/hyundai/in/en/data/find-a-car/Grand-i10-Nios/Gallery%20Section/big/pc/niosgallery_3.jpg</t>
   </si>
   <si>
     <t>https://www.hyundai.com/in/en/find-a-car/grand-i10-nios/highlights</t>
@@ -658,16 +646,10 @@
     <t>Mahindra BE 6 FE</t>
   </si>
   <si>
-    <t>https://stimg.cardekho.com/images/carexteriorimages/630x420/Mahindra/BE-6/9263/1762423834412/front-left-side-47.jpg</t>
-  </si>
-  <si>
     <t>https://www.mahindraelectricsuv.com/esuv/be-6/MBE6.html</t>
   </si>
   <si>
     <t>https://www.mahindraelectricsuv.com/esuv/xev-9e/MXV9.html</t>
-  </si>
-  <si>
-    <t>https://car.zigcdn.com/images/car-images/360x240/Mahindra-XEV/9e/9262/1732783821808/226_Mahindra-XEV-9e_Deep-Forest_42413d.jpg</t>
   </si>
   <si>
     <t>https://imgd.aeplcdn.com/664x374/n/cw/ec/212003/xev9s-exterior-right-front-three-quarter-11.png?isig=0&amp;q=80</t>
@@ -841,9 +823,6 @@
     <t>https://cars.tatamotors.com/punch/ice/register-interest.html</t>
   </si>
   <si>
-    <t>https://stimg.cardekho.com/images/carexteriorimages/930x620/Tata/Punch/9623/1762425519212/front-left-side-47.jpg</t>
-  </si>
-  <si>
     <t>Tata Punch EV</t>
   </si>
   <si>
@@ -974,6 +953,27 @@
   </si>
   <si>
     <t>fuel_ev</t>
+  </si>
+  <si>
+    <t>Hyundai VENUE N LINE</t>
+  </si>
+  <si>
+    <t>https://www.hyundai.com/content/dam/hyundai/in/en/data/find-a-car/Venue/360/mystic-sapphire/pc/mystic-sapphire_5.png</t>
+  </si>
+  <si>
+    <t>https://www.hyundai.com/content/dam/hyundai/in/en/data/find-a-car/Exter/360/knight-black/pc/knight-black_5.png</t>
+  </si>
+  <si>
+    <t>https://www.hyundai.com/content/dam/hyundai/in/en/data/find-a-car/Grand-i10-Nios/360/fiery-red/pc/fiery-red_6.png</t>
+  </si>
+  <si>
+    <t>https://www.mahindraelectricsuv.com/dw/image/v2/BKRC_PRD/on/demandware.static/-/Sites-esuv-product-catalog/default/dw2d1c2f73/images/BE6/large/packtwo/Everest_White_Matte_588x330.png</t>
+  </si>
+  <si>
+    <t>https://www.mahindraelectricsuv.com/dw/image/v2/BKRC_PRD/on/demandware.static/-/Sites-esuv-product-catalog/default/dwfd97cd9b/images/XEV9E/large/packtwo/Tango_Red_588x330.png</t>
+  </si>
+  <si>
+    <t>https://s7ap1.scene7.com/is/image/tatamotors/punch-mce-navigation?$HC-264-129-D$&amp;fit=fit&amp;fmt=avif-alpha</t>
   </si>
 </sst>
 </file>
@@ -1369,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24CD22A1-0E23-6F4B-BCA3-DE3CB9046986}">
   <dimension ref="A1:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X48" sqref="X48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1429,10 +1429,10 @@
         <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>24</v>
@@ -1447,19 +1447,19 @@
         <v>23</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>17</v>
@@ -1471,7 +1471,7 @@
         <v>20</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>4</v>
@@ -1554,7 +1554,7 @@
         <v>0</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="Y2" s="2" t="s">
         <v>21</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="3" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
@@ -1634,24 +1634,24 @@
         <v>0</v>
       </c>
       <c r="X3" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="Y3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="119" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>82</v>
+        <v>302</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
@@ -1714,24 +1714,24 @@
         <v>0</v>
       </c>
       <c r="X4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="Y4" s="2" t="s">
+      <c r="Z4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="Z4" s="1" t="s">
-        <v>80</v>
-      </c>
     </row>
-    <row r="5" spans="1:26" ht="85" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
@@ -1794,24 +1794,24 @@
         <v>0</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>83</v>
+        <v>304</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
@@ -1874,24 +1874,24 @@
         <v>0</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="119" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
@@ -1954,27 +1954,27 @@
         <v>0</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="119" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -2034,27 +2034,27 @@
         <v>0</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>94</v>
+        <v>305</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -2114,27 +2114,27 @@
         <v>0</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="Y9" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
@@ -2194,27 +2194,27 @@
         <v>0</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="Y10" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -2274,27 +2274,27 @@
         <v>0</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="Z11" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -2354,24 +2354,24 @@
         <v>0</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
@@ -2419,7 +2419,7 @@
         <v>5</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="T13" s="1">
         <v>1</v>
@@ -2434,24 +2434,24 @@
         <v>0</v>
       </c>
       <c r="X13" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y13" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="Y13" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="Z13" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
@@ -2514,27 +2514,27 @@
         <v>0</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="Y14" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -2594,27 +2594,27 @@
         <v>1</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="Y15" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
@@ -2674,27 +2674,27 @@
         <v>1</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="Y16" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:26" ht="187" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E17" s="1">
         <v>1</v>
@@ -2754,24 +2754,24 @@
         <v>0</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="Z17" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>8</v>
@@ -2834,27 +2834,27 @@
         <v>0</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="Y18" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="Z18" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="170" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
@@ -2914,27 +2914,27 @@
         <v>0</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="Y19" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="Z19" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:26" ht="221" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -2994,27 +2994,27 @@
         <v>0</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="Y20" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="Z20" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>
@@ -3074,24 +3074,24 @@
         <v>0</v>
       </c>
       <c r="X21" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="Y21" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="Z21" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>8</v>
@@ -3154,24 +3154,24 @@
         <v>0</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="Z22" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>8</v>
@@ -3234,24 +3234,24 @@
         <v>0</v>
       </c>
       <c r="X23" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="Y23" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="Z23" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>8</v>
@@ -3314,24 +3314,24 @@
         <v>0</v>
       </c>
       <c r="X24" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="Y24" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="Z24" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>8</v>
@@ -3394,24 +3394,24 @@
         <v>0</v>
       </c>
       <c r="X25" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="Z25" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>8</v>
@@ -3474,24 +3474,24 @@
         <v>0</v>
       </c>
       <c r="X26" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="Y26" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="Z26" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>8</v>
@@ -3554,24 +3554,24 @@
         <v>0</v>
       </c>
       <c r="X27" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="Y27" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="Z27" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>8</v>
@@ -3634,24 +3634,24 @@
         <v>0</v>
       </c>
       <c r="X28" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="Y28" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="Z28" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>8</v>
@@ -3714,24 +3714,24 @@
         <v>0</v>
       </c>
       <c r="X29" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="Y29" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="Z29" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" spans="1:26" ht="119" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>8</v>
@@ -3794,24 +3794,24 @@
         <v>0</v>
       </c>
       <c r="X30" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="Y30" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="Z30" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:26" ht="170" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>8</v>
@@ -3874,24 +3874,24 @@
         <v>0</v>
       </c>
       <c r="X31" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="Y31" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="Z31" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>8</v>
@@ -3954,24 +3954,24 @@
         <v>0</v>
       </c>
       <c r="X32" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="Y32" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="Z32" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
-    <row r="33" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>8</v>
@@ -4034,24 +4034,24 @@
         <v>0</v>
       </c>
       <c r="X33" s="2" t="s">
-        <v>205</v>
+        <v>306</v>
       </c>
       <c r="Y33" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="Z33" s="1" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
-    <row r="34" spans="1:26" ht="136" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>8</v>
@@ -4114,24 +4114,24 @@
         <v>0</v>
       </c>
       <c r="X34" s="2" t="s">
-        <v>208</v>
+        <v>307</v>
       </c>
       <c r="Y34" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="Z34" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>8</v>
@@ -4194,24 +4194,24 @@
         <v>0</v>
       </c>
       <c r="X35" s="2" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="Y35" s="2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="Z35" s="1" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>8</v>
@@ -4274,27 +4274,27 @@
         <v>0</v>
       </c>
       <c r="X36" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="Y36" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="Z36" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="37" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E37" s="1">
         <v>1</v>
@@ -4354,27 +4354,27 @@
         <v>1</v>
       </c>
       <c r="X37" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="Y37" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="Z37" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E38" s="1">
         <v>1</v>
@@ -4434,27 +4434,27 @@
         <v>1</v>
       </c>
       <c r="X38" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="Y38" s="2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="Z38" s="1" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:26" ht="119" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E39" s="1">
         <v>1</v>
@@ -4514,27 +4514,27 @@
         <v>1</v>
       </c>
       <c r="X39" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="Y39" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="Z39" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -4594,27 +4594,27 @@
         <v>1</v>
       </c>
       <c r="X40" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="Y40" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="Z40" s="1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E41" s="1">
         <v>1</v>
@@ -4674,27 +4674,27 @@
         <v>1</v>
       </c>
       <c r="X41" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="Y41" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="Z41" s="1" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="42" spans="1:26" ht="68" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E42" s="1">
         <v>1</v>
@@ -4754,27 +4754,27 @@
         <v>0</v>
       </c>
       <c r="X42" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="Y42" s="1" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="Z42" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="43" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E43" s="1">
         <v>0</v>
@@ -4834,27 +4834,27 @@
         <v>0</v>
       </c>
       <c r="X43" s="2" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="Y43" s="2" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="Z43" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="44" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E44" s="1">
         <v>1</v>
@@ -4914,27 +4914,27 @@
         <v>0</v>
       </c>
       <c r="X44" s="2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="Y44" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="Z44" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="45" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E45" s="1">
         <v>1</v>
@@ -4994,27 +4994,27 @@
         <v>0</v>
       </c>
       <c r="X45" s="2" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="Y45" s="2" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="Z45" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="46" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
@@ -5074,27 +5074,27 @@
         <v>0</v>
       </c>
       <c r="X46" s="2" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="Y46" s="2" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="Z46" s="1" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="47" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E47" s="1">
         <v>1</v>
@@ -5154,24 +5154,24 @@
         <v>0</v>
       </c>
       <c r="X47" s="2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="Y47" s="2" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="Z47" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
-    <row r="48" spans="1:26" ht="85" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>8</v>
@@ -5234,24 +5234,24 @@
         <v>0</v>
       </c>
       <c r="X48" s="2" t="s">
-        <v>265</v>
+        <v>308</v>
       </c>
       <c r="Y48" s="2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="Z48" s="1" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="49" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>8</v>
@@ -5314,24 +5314,24 @@
         <v>0</v>
       </c>
       <c r="X49" s="2" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="Y49" s="2" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="Z49" s="1" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="50" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>8</v>
@@ -5394,24 +5394,24 @@
         <v>0</v>
       </c>
       <c r="X50" s="2" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="Y50" s="2" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="Z50" s="1" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="51" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>8</v>
@@ -5474,24 +5474,24 @@
         <v>0</v>
       </c>
       <c r="X51" s="2" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="Y51" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="Z51" s="1" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="52" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>8</v>
@@ -5554,24 +5554,24 @@
         <v>0</v>
       </c>
       <c r="X52" s="2" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="Y52" s="2" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="Z52" s="1" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
     </row>
     <row r="53" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>287</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>8</v>
@@ -5634,24 +5634,24 @@
         <v>0</v>
       </c>
       <c r="X53" s="2" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="Y53" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="Z53" s="1" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
     <row r="54" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>8</v>
@@ -5714,24 +5714,24 @@
         <v>0</v>
       </c>
       <c r="X54" s="2" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="Y54" s="2" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="Z54" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="55" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>8</v>
@@ -5794,24 +5794,24 @@
         <v>0</v>
       </c>
       <c r="X55" s="2" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="Y55" s="2" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="Z55" s="1" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
     </row>
     <row r="56" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>8</v>
@@ -5874,13 +5874,13 @@
         <v>0</v>
       </c>
       <c r="X56" s="2" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="Y56" s="2" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="Z56" s="1" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Report section Update - Car combination Doesn't exist
</commit_message>
<xml_diff>
--- a/Backend/car_data.xlsx
+++ b/Backend/car_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rishabhsurana/Desktop/Rishabh/CarGo.com/CarAdvisor-AI/Backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C8D93F-5D34-4743-8626-8E459BD535C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9438440B-1B91-234B-86E5-4DF8A3F0FD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{FCCC8226-0F48-1143-B6BE-845B3E6942EE}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="17340" xr2:uid="{FCCC8226-0F48-1143-B6BE-845B3E6942EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,9 +428,6 @@
     <t>Hyundai PRIME SD</t>
   </si>
   <si>
-    <t>https://www.hyundai.com/content/dam/hyundai/in/en/data/home/homemodel-venue.png</t>
-  </si>
-  <si>
     <t>Honda</t>
   </si>
   <si>
@@ -974,6 +971,9 @@
   </si>
   <si>
     <t>https://s7ap1.scene7.com/is/image/tatamotors/punch-mce-navigation?$HC-264-129-D$&amp;fit=fit&amp;fmt=avif-alpha</t>
+  </si>
+  <si>
+    <t>https://www.hyundai.com/content/dam/hyundai/in/en/data/find-a-car/Creta/360/abyss-black/pc/abyss-black_6.png</t>
   </si>
 </sst>
 </file>
@@ -1369,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24CD22A1-0E23-6F4B-BCA3-DE3CB9046986}">
   <dimension ref="A1:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X48" sqref="X48"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1429,10 +1429,10 @@
         <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>301</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>24</v>
@@ -1447,19 +1447,19 @@
         <v>23</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>299</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>17</v>
@@ -1554,7 +1554,7 @@
         <v>0</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>130</v>
+        <v>308</v>
       </c>
       <c r="Y2" s="2" t="s">
         <v>21</v>
@@ -1634,7 +1634,7 @@
         <v>0</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="Y3" s="1" t="s">
         <v>26</v>
@@ -1651,7 +1651,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
@@ -1794,7 +1794,7 @@
         <v>0</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="Y5" s="2" t="s">
         <v>81</v>
@@ -2034,7 +2034,7 @@
         <v>0</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Y8" s="2" t="s">
         <v>91</v>
@@ -2688,10 +2688,10 @@
         <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>104</v>
@@ -2754,13 +2754,13 @@
         <v>0</v>
       </c>
       <c r="X17" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z17" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="Y17" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="Z17" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:26" ht="153" x14ac:dyDescent="0.2">
@@ -2768,10 +2768,10 @@
         <v>43</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>8</v>
@@ -2834,13 +2834,13 @@
         <v>0</v>
       </c>
       <c r="X18" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y18" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="Y18" s="2" t="s">
+      <c r="Z18" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="Z18" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="170" x14ac:dyDescent="0.2">
@@ -2848,10 +2848,10 @@
         <v>44</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>104</v>
@@ -2914,13 +2914,13 @@
         <v>0</v>
       </c>
       <c r="X19" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y19" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="Y19" s="2" t="s">
+      <c r="Z19" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="Z19" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:26" ht="221" x14ac:dyDescent="0.2">
@@ -2928,10 +2928,10 @@
         <v>45</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>104</v>
@@ -2994,13 +2994,13 @@
         <v>0</v>
       </c>
       <c r="X20" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y20" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="Y20" s="2" t="s">
+      <c r="Z20" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="Z20" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:26" ht="153" x14ac:dyDescent="0.2">
@@ -3008,10 +3008,10 @@
         <v>46</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>104</v>
@@ -3074,13 +3074,13 @@
         <v>0</v>
       </c>
       <c r="X21" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="Y21" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z21" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="Z21" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:26" ht="136" x14ac:dyDescent="0.2">
@@ -3088,10 +3088,10 @@
         <v>47</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>8</v>
@@ -3154,13 +3154,13 @@
         <v>0</v>
       </c>
       <c r="X22" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y22" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="Y22" s="2" t="s">
+      <c r="Z22" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="Z22" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:26" ht="136" x14ac:dyDescent="0.2">
@@ -3168,10 +3168,10 @@
         <v>48</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>8</v>
@@ -3234,13 +3234,13 @@
         <v>0</v>
       </c>
       <c r="X23" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="Y23" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="Y23" s="2" t="s">
+      <c r="Z23" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="Z23" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="136" x14ac:dyDescent="0.2">
@@ -3248,10 +3248,10 @@
         <v>49</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>8</v>
@@ -3314,13 +3314,13 @@
         <v>0</v>
       </c>
       <c r="X24" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y24" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="Y24" s="2" t="s">
+      <c r="Z24" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="Z24" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:26" ht="136" x14ac:dyDescent="0.2">
@@ -3328,10 +3328,10 @@
         <v>50</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>8</v>
@@ -3394,13 +3394,13 @@
         <v>0</v>
       </c>
       <c r="X25" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="Y25" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z25" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="Y25" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="Z25" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:26" ht="136" x14ac:dyDescent="0.2">
@@ -3408,10 +3408,10 @@
         <v>51</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>8</v>
@@ -3474,13 +3474,13 @@
         <v>0</v>
       </c>
       <c r="X26" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="Y26" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="Y26" s="2" t="s">
+      <c r="Z26" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="Z26" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:26" ht="136" x14ac:dyDescent="0.2">
@@ -3488,10 +3488,10 @@
         <v>52</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>8</v>
@@ -3554,13 +3554,13 @@
         <v>0</v>
       </c>
       <c r="X27" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="Y27" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="Y27" s="2" t="s">
+      <c r="Z27" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="Z27" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:26" ht="136" x14ac:dyDescent="0.2">
@@ -3568,10 +3568,10 @@
         <v>53</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>8</v>
@@ -3634,13 +3634,13 @@
         <v>0</v>
       </c>
       <c r="X28" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="Y28" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="Y28" s="2" t="s">
+      <c r="Z28" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="Z28" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:26" ht="136" x14ac:dyDescent="0.2">
@@ -3648,10 +3648,10 @@
         <v>54</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>8</v>
@@ -3714,13 +3714,13 @@
         <v>0</v>
       </c>
       <c r="X29" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y29" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="Y29" s="2" t="s">
+      <c r="Z29" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="Z29" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="30" spans="1:26" ht="119" x14ac:dyDescent="0.2">
@@ -3728,10 +3728,10 @@
         <v>55</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>8</v>
@@ -3794,13 +3794,13 @@
         <v>0</v>
       </c>
       <c r="X30" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y30" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="Y30" s="2" t="s">
+      <c r="Z30" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="Z30" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:26" ht="170" x14ac:dyDescent="0.2">
@@ -3808,10 +3808,10 @@
         <v>56</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>8</v>
@@ -3874,13 +3874,13 @@
         <v>0</v>
       </c>
       <c r="X31" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y31" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="Y31" s="2" t="s">
+      <c r="Z31" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="Z31" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:26" ht="153" x14ac:dyDescent="0.2">
@@ -3888,10 +3888,10 @@
         <v>57</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>8</v>
@@ -3954,13 +3954,13 @@
         <v>0</v>
       </c>
       <c r="X32" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="Y32" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="Y32" s="2" t="s">
+      <c r="Z32" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="Z32" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="33" spans="1:26" ht="153" x14ac:dyDescent="0.2">
@@ -3968,10 +3968,10 @@
         <v>58</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>8</v>
@@ -4034,13 +4034,13 @@
         <v>0</v>
       </c>
       <c r="X33" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Y33" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Z33" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:26" ht="153" x14ac:dyDescent="0.2">
@@ -4048,10 +4048,10 @@
         <v>59</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>8</v>
@@ -4114,13 +4114,13 @@
         <v>0</v>
       </c>
       <c r="X34" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Y34" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Z34" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:26" ht="85" x14ac:dyDescent="0.2">
@@ -4128,10 +4128,10 @@
         <v>60</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>8</v>
@@ -4194,13 +4194,13 @@
         <v>0</v>
       </c>
       <c r="X35" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y35" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="Y35" s="2" t="s">
+      <c r="Z35" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="Z35" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="136" x14ac:dyDescent="0.2">
@@ -4208,10 +4208,10 @@
         <v>61</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>8</v>
@@ -4274,13 +4274,13 @@
         <v>0</v>
       </c>
       <c r="X36" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Y36" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z36" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:26" ht="153" x14ac:dyDescent="0.2">
@@ -4288,13 +4288,13 @@
         <v>62</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="E37" s="1">
         <v>1</v>
@@ -4354,13 +4354,13 @@
         <v>1</v>
       </c>
       <c r="X37" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="Y37" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="Y37" s="2" t="s">
+      <c r="Z37" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="Z37" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:26" ht="136" x14ac:dyDescent="0.2">
@@ -4368,13 +4368,13 @@
         <v>63</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E38" s="1">
         <v>1</v>
@@ -4434,13 +4434,13 @@
         <v>1</v>
       </c>
       <c r="X38" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Y38" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="Y38" s="2" t="s">
+      <c r="Z38" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="Z38" s="1" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:26" ht="119" x14ac:dyDescent="0.2">
@@ -4448,13 +4448,13 @@
         <v>64</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E39" s="1">
         <v>1</v>
@@ -4514,13 +4514,13 @@
         <v>1</v>
       </c>
       <c r="X39" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y39" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="Y39" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="Z39" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="1:26" ht="153" x14ac:dyDescent="0.2">
@@ -4528,13 +4528,13 @@
         <v>65</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -4594,13 +4594,13 @@
         <v>1</v>
       </c>
       <c r="X40" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="Y40" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="Z40" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="Y40" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="Z40" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:26" ht="153" x14ac:dyDescent="0.2">
@@ -4608,13 +4608,13 @@
         <v>66</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E41" s="1">
         <v>1</v>
@@ -4674,13 +4674,13 @@
         <v>1</v>
       </c>
       <c r="X41" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="Y41" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="Y41" s="2" t="s">
-        <v>229</v>
-      </c>
       <c r="Z41" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="42" spans="1:26" ht="68" x14ac:dyDescent="0.2">
@@ -4688,10 +4688,10 @@
         <v>67</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>104</v>
@@ -4754,13 +4754,13 @@
         <v>0</v>
       </c>
       <c r="X42" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Y42" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Z42" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="43" spans="1:26" ht="102" x14ac:dyDescent="0.2">
@@ -4768,10 +4768,10 @@
         <v>68</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>104</v>
@@ -4834,13 +4834,13 @@
         <v>0</v>
       </c>
       <c r="X43" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="Y43" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="Y43" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="Z43" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="44" spans="1:26" ht="102" x14ac:dyDescent="0.2">
@@ -4848,10 +4848,10 @@
         <v>69</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>94</v>
@@ -4914,13 +4914,13 @@
         <v>0</v>
       </c>
       <c r="X44" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="Y44" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="Y44" s="1" t="s">
+      <c r="Z44" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="Z44" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="45" spans="1:26" ht="102" x14ac:dyDescent="0.2">
@@ -4928,10 +4928,10 @@
         <v>70</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>94</v>
@@ -4994,13 +4994,13 @@
         <v>0</v>
       </c>
       <c r="X45" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y45" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="Y45" s="2" t="s">
+      <c r="Z45" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="Z45" s="1" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="46" spans="1:26" ht="102" x14ac:dyDescent="0.2">
@@ -5008,10 +5008,10 @@
         <v>71</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>94</v>
@@ -5074,13 +5074,13 @@
         <v>0</v>
       </c>
       <c r="X46" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Y46" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="Z46" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="Y46" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="Z46" s="1" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="47" spans="1:26" ht="102" x14ac:dyDescent="0.2">
@@ -5088,10 +5088,10 @@
         <v>72</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>94</v>
@@ -5154,13 +5154,13 @@
         <v>0</v>
       </c>
       <c r="X47" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="Y47" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="Z47" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="Y47" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="Z47" s="1" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="48" spans="1:26" ht="102" x14ac:dyDescent="0.2">
@@ -5168,10 +5168,10 @@
         <v>73</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>8</v>
@@ -5234,13 +5234,13 @@
         <v>0</v>
       </c>
       <c r="X48" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Y48" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Z48" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="49" spans="1:26" ht="102" x14ac:dyDescent="0.2">
@@ -5248,10 +5248,10 @@
         <v>74</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>8</v>
@@ -5314,13 +5314,13 @@
         <v>0</v>
       </c>
       <c r="X49" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="Y49" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="Z49" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="Y49" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="Z49" s="1" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="50" spans="1:26" ht="102" x14ac:dyDescent="0.2">
@@ -5328,10 +5328,10 @@
         <v>75</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>8</v>
@@ -5394,13 +5394,13 @@
         <v>0</v>
       </c>
       <c r="X50" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="Y50" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="Y50" s="2" t="s">
-        <v>267</v>
-      </c>
       <c r="Z50" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="51" spans="1:26" ht="102" x14ac:dyDescent="0.2">
@@ -5408,10 +5408,10 @@
         <v>76</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>8</v>
@@ -5474,24 +5474,24 @@
         <v>0</v>
       </c>
       <c r="X51" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="Y51" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="Y51" s="2" t="s">
+      <c r="Z51" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="Z51" s="1" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="52" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>8</v>
@@ -5554,24 +5554,24 @@
         <v>0</v>
       </c>
       <c r="X52" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="Y52" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="Z52" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="Y52" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="Z52" s="1" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="53" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>8</v>
@@ -5634,24 +5634,24 @@
         <v>0</v>
       </c>
       <c r="X53" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="Y53" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="Y53" s="2" t="s">
+      <c r="Z53" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="Z53" s="1" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="54" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>8</v>
@@ -5714,24 +5714,24 @@
         <v>0</v>
       </c>
       <c r="X54" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="Y54" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="Z54" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="Y54" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="Z54" s="1" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="55" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>8</v>
@@ -5794,24 +5794,24 @@
         <v>0</v>
       </c>
       <c r="X55" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="Y55" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="Y55" s="2" t="s">
+      <c r="Z55" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="Z55" s="1" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="56" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>8</v>
@@ -5874,13 +5874,13 @@
         <v>0</v>
       </c>
       <c r="X56" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="Y56" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="Z56" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="Y56" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="Z56" s="1" t="s">
-        <v>296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backend - JSON for findcar update
</commit_message>
<xml_diff>
--- a/Backend/car_data.xlsx
+++ b/Backend/car_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rishabhsurana/Desktop/Rishabh/CarGo.com/CarAdvisor-AI/Backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9438440B-1B91-234B-86E5-4DF8A3F0FD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1944A5-D668-004B-93B2-619799C36122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="17340" xr2:uid="{FCCC8226-0F48-1143-B6BE-845B3E6942EE}"/>
   </bookViews>
@@ -1369,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24CD22A1-0E23-6F4B-BCA3-DE3CB9046986}">
   <dimension ref="A1:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>